<commit_message>
First complete draft, with many questions
</commit_message>
<xml_diff>
--- a/fielddescriptions.xlsx
+++ b/fielddescriptions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\electionresults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\electionresultsparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6437D495-C199-4C50-AEF3-5FF2FAB928BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{6B46DF32-5C05-488C-A1B0-41430B5314BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{6B46DF32-5C05-488C-A1B0-41430B5314BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -146,18 +147,12 @@
     <t>winner</t>
   </si>
   <si>
-    <t>FieldName</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Unique race ID for a specific state</t>
   </si>
   <si>
-    <t>Character string indicating the type of race (for example, GOP Primary, General, Democratic Caucus)</t>
-  </si>
-  <si>
     <t>Single-character race type ID D (Dem Primary), R (GOP Primary), G (General), E (Dem Caucus), S (GOP Caucus)</t>
   </si>
   <si>
@@ -197,9 +192,6 @@
     <t>Candidate's last name</t>
   </si>
   <si>
-    <t>Date of the election day, in format m/d/yyyy</t>
-  </si>
-  <si>
     <t>Time last updated. Sample: 2018-03-07T17:24:47.600Z</t>
   </si>
   <si>
@@ -207,6 +199,132 @@
   </si>
   <si>
     <t>Indicates that the race is national. "TRUE"</t>
+  </si>
+  <si>
+    <t>FieldName - CSV</t>
+  </si>
+  <si>
+    <t>FieldName - JSON</t>
+  </si>
+  <si>
+    <t>raceID</t>
+  </si>
+  <si>
+    <t>RaceType</t>
+  </si>
+  <si>
+    <t>Character string indicating the type of race (for example, GOP Primary, General, Democratic Caucus). Sample: "Primary"</t>
+  </si>
+  <si>
+    <t>raceTypeID</t>
+  </si>
+  <si>
+    <t>officeID</t>
+  </si>
+  <si>
+    <t>polID</t>
+  </si>
+  <si>
+    <t>officeName</t>
+  </si>
+  <si>
+    <t>polNum</t>
+  </si>
+  <si>
+    <t>ballotOrder</t>
+  </si>
+  <si>
+    <t>candidateID</t>
+  </si>
+  <si>
+    <t>electionDate</t>
+  </si>
+  <si>
+    <t>Date of the election day, in format m/d/yyyy in CSV; in JSON, yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>fipsCode</t>
+  </si>
+  <si>
+    <t>In JSON, if present, marked with "X"</t>
+  </si>
+  <si>
+    <t>precinctsReporting</t>
+  </si>
+  <si>
+    <t>precinctsTotal</t>
+  </si>
+  <si>
+    <t>precinctsReportingPct</t>
+  </si>
+  <si>
+    <t>In CSV, 100% = 1. In JSON, 100%=100.0.</t>
+  </si>
+  <si>
+    <t>reportingunitID</t>
+  </si>
+  <si>
+    <t>reportingunitName</t>
+  </si>
+  <si>
+    <t>seatName</t>
+  </si>
+  <si>
+    <t>stateName</t>
+  </si>
+  <si>
+    <t>Note JSON capitalization</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>Sample: "2018-10-04T22:11:18.413Z"</t>
+  </si>
+  <si>
+    <t>e.g, "Arizona"</t>
+  </si>
+  <si>
+    <t>statePostal</t>
+  </si>
+  <si>
+    <t>e.g., "AZ"</t>
+  </si>
+  <si>
+    <t>JSON example: "false"</t>
+  </si>
+  <si>
+    <t>In CSV, 100% = 1. In JSON, absent.</t>
+  </si>
+  <si>
+    <t>Office type ID, usually a single character: for example: P (President), G (Governor), S (U.S. Senate), H (U.S. House)</t>
+  </si>
+  <si>
+    <t>Name of the office, ballot initiative or other race</t>
+  </si>
+  <si>
+    <t>Party abbreviation (or example, Dem, GOP, Lib). This field is not applicable to a general election race. It is applicable to the closed primaries where there is more than one race for the same office, for example, Dem Governor race and GOP Governor race.</t>
+  </si>
+  <si>
+    <t>Unique national politician ID across all states and races (only for politicians who have run in a national race). For local politicians, this value is set to "0"</t>
+  </si>
+  <si>
+    <t>Current number of votes for a particular candidate</t>
+  </si>
+  <si>
+    <t>E.g., "District 4"</t>
+  </si>
+  <si>
+    <t>E.g., "4"</t>
+  </si>
+  <si>
+    <t>seatNum</t>
+  </si>
+  <si>
+    <t>nextrequest</t>
+  </si>
+  <si>
+    <t>URL for next hit to AP servers for data via Elex</t>
   </si>
 </sst>
 </file>
@@ -568,288 +686,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FAB618-7688-4A0E-8FF4-867B22C49E77}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="1" max="2" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>39</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Some Git weirdness"
This reverts commit 326398542dfef247b00dc17ba8789faa4ed3e52a, reversing
changes made to 49940df882eb40c84948f3bd11ff15902f6b53db.
</commit_message>
<xml_diff>
--- a/fielddescriptions.xlsx
+++ b/fielddescriptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\election-results-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\electionresultsparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854F5239-2B47-4D1C-9E24-0D919E5DE784}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6437D495-C199-4C50-AEF3-5FF2FAB928BD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" xr2:uid="{6B46DF32-5C05-488C-A1B0-41430B5314BD}"/>
   </bookViews>

</xml_diff>